<commit_message>
convert cost by GDP for fl risk
</commit_message>
<xml_diff>
--- a/output/damage/PHL_osm_fl_historical_damage_1.xlsx
+++ b/output/damage/PHL_osm_fl_historical_damage_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F1_1_1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4404783.63313817</v>
+        <v>199863.9019834792</v>
       </c>
       <c r="F2" t="n">
-        <v>3303587.724853627</v>
+        <v>149897.9264876094</v>
       </c>
       <c r="G2" t="n">
-        <v>5505979.541422713</v>
+        <v>249829.877479349</v>
       </c>
     </row>
     <row r="3">
@@ -505,22 +505,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F1_1_2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>265802.1384990234</v>
+        <v>1005062.725491634</v>
       </c>
       <c r="F3" t="n">
-        <v>199351.6038742675</v>
+        <v>753797.0441187255</v>
       </c>
       <c r="G3" t="n">
-        <v>332252.6731237792</v>
+        <v>1256328.406864542</v>
       </c>
     </row>
     <row r="4">
@@ -529,12 +529,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>rp0002</t>
+          <t>rp0001</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F1_1_3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4772232.913539903</v>
+        <v>1005062.725491634</v>
       </c>
       <c r="F4" t="n">
-        <v>3579174.685154927</v>
+        <v>753797.0441187255</v>
       </c>
       <c r="G4" t="n">
-        <v>5965291.141924879</v>
+        <v>1256328.406864542</v>
       </c>
     </row>
     <row r="5">
@@ -558,12 +558,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>rp0002</t>
+          <t>rp0001</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F2_1_1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>265802.1384990234</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>199351.6038742675</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>332252.6731237792</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -587,27 +587,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>rp0005</t>
+          <t>rp0001</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F2_1_2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>5591933.769316998</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>4193950.326987748</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>6989917.211646249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -616,12 +616,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rp0005</t>
+          <t>rp0001</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F2_1_3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -630,13 +630,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>265802.1384990234</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>199351.6038742675</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>332252.6731237792</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -645,12 +645,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>rp0010</t>
+          <t>rp0002</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F1_1_1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>6212590.267201408</v>
+        <v>226155.7457910703</v>
       </c>
       <c r="F8" t="n">
-        <v>4659442.700401054</v>
+        <v>169616.8093433026</v>
       </c>
       <c r="G8" t="n">
-        <v>7765737.834001759</v>
+        <v>282694.6822388378</v>
       </c>
     </row>
     <row r="9">
@@ -674,27 +674,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>rp0010</t>
+          <t>rp0002</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F1_1_2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>265802.1384990234</v>
+        <v>1137277.457282681</v>
       </c>
       <c r="F9" t="n">
-        <v>199351.6038742675</v>
+        <v>852958.0929620105</v>
       </c>
       <c r="G9" t="n">
-        <v>332252.6731237792</v>
+        <v>1421596.821603351</v>
       </c>
     </row>
     <row r="10">
@@ -703,12 +703,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>rp0025</t>
+          <t>rp0002</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F1_1_3</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>7356821.379866531</v>
+        <v>1137277.457282681</v>
       </c>
       <c r="F10" t="n">
-        <v>5517616.034899896</v>
+        <v>852958.0929620105</v>
       </c>
       <c r="G10" t="n">
-        <v>9196026.724833163</v>
+        <v>1421596.821603351</v>
       </c>
     </row>
     <row r="11">
@@ -732,12 +732,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>rp0025</t>
+          <t>rp0002</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F2_1_1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -746,13 +746,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>265802.1384990234</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>199351.6038742675</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>332252.6731237792</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -761,27 +761,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>rp0050</t>
+          <t>rp0002</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F2_1_2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>8595913.607487826</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>6446935.205615868</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>10744892.00935978</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -790,12 +790,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>rp0050</t>
+          <t>rp0002</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F2_1_3</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>265802.1384990234</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>199351.6038742675</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>332252.6731237792</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -819,12 +819,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>rp0100</t>
+          <t>rp0005</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F1_1_1</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>11097253.48905634</v>
+        <v>289053.8236105831</v>
       </c>
       <c r="F14" t="n">
-        <v>8322940.116792252</v>
+        <v>216790.3677079373</v>
       </c>
       <c r="G14" t="n">
-        <v>13871566.86132042</v>
+        <v>361317.2795132289</v>
       </c>
     </row>
     <row r="15">
@@ -848,27 +848,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>rp0100</t>
+          <t>rp0005</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F1_1_2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1082720.624889485</v>
+        <v>1453575.262409541</v>
       </c>
       <c r="F15" t="n">
-        <v>812040.4686671138</v>
+        <v>1090181.446807156</v>
       </c>
       <c r="G15" t="n">
-        <v>1353400.781111856</v>
+        <v>1816969.078011927</v>
       </c>
     </row>
     <row r="16">
@@ -877,12 +877,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>rp0250</t>
+          <t>rp0005</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F1_1_3</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -891,13 +891,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>15546963.42773451</v>
+        <v>1453575.262409541</v>
       </c>
       <c r="F16" t="n">
-        <v>11660222.57080088</v>
+        <v>1090181.446807156</v>
       </c>
       <c r="G16" t="n">
-        <v>19433704.28466813</v>
+        <v>1816969.078011927</v>
       </c>
     </row>
     <row r="17">
@@ -906,12 +906,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>rp0250</t>
+          <t>rp0005</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F2_1_1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -920,13 +920,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3200029.141303625</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>2400021.855977718</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>4000036.426629531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -935,27 +935,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>rp0500</t>
+          <t>rp0005</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F2_1_2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>substation</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>19116823.17305563</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>14337617.37979172</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>23896028.96631954</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -964,12 +964,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>rp0500</t>
+          <t>rp0005</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>substation</t>
+          <t>F2_1_3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>4424089.405760903</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>3318067.054320677</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>5530111.757201129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -993,12 +993,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>rp1000</t>
+          <t>rp0010</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>F1_1_1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1007,13 +1007,13 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>23860130.80766758</v>
+        <v>351658.4867713291</v>
       </c>
       <c r="F20" t="n">
-        <v>17895098.10575068</v>
+        <v>263743.8650784967</v>
       </c>
       <c r="G20" t="n">
-        <v>29825163.50958448</v>
+        <v>439573.1084641614</v>
       </c>
     </row>
     <row r="21">
@@ -1022,27 +1022,1187 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>rp0010</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>F1_1_2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>1768397.562786856</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1326298.172090142</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2210496.95348357</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>rp0010</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>F1_1_3</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>1768397.562786856</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1326298.172090142</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2210496.95348357</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>rp0010</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>F2_1_1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>rp0010</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>F2_1_2</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>rp0010</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>F2_1_3</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>F1_1_1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>429816.0241677746</v>
+      </c>
+      <c r="F26" t="n">
+        <v>322362.0181258308</v>
+      </c>
+      <c r="G26" t="n">
+        <v>537270.0302097183</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>F1_1_2</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>2161431.156016107</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1621073.367012081</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2701788.945020135</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>F1_1_3</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>2161431.156016107</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1621073.367012081</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2701788.945020135</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>F2_1_1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>F2_1_2</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>rp0025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>F2_1_3</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>F1_1_1</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>541716.5514298822</v>
+      </c>
+      <c r="F32" t="n">
+        <v>406287.4135724115</v>
+      </c>
+      <c r="G32" t="n">
+        <v>677145.6892873528</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>F1_1_2</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>2724149.324719235</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2043111.993539426</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3405186.655899044</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>F1_1_3</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>2724149.324719235</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2043111.993539426</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3405186.655899044</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>F2_1_1</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>F2_1_2</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>rp0050</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>F2_1_3</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>F1_1_1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>721512.0403776906</v>
+      </c>
+      <c r="F38" t="n">
+        <v>541134.0302832677</v>
+      </c>
+      <c r="G38" t="n">
+        <v>901890.0504721131</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>F1_1_2</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>3628293.306497007</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2721219.979872755</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4535366.633121259</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>F1_1_3</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>3628293.306497007</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2721219.979872755</v>
+      </c>
+      <c r="G40" t="n">
+        <v>4535366.633121259</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>F2_1_1</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>11818.25183344388</v>
+      </c>
+      <c r="F41" t="n">
+        <v>8863.688875082909</v>
+      </c>
+      <c r="G41" t="n">
+        <v>14772.81479180485</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>F2_1_2</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>23636.50366688776</v>
+      </c>
+      <c r="F42" t="n">
+        <v>17727.37775016582</v>
+      </c>
+      <c r="G42" t="n">
+        <v>29545.62958360969</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>rp0100</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>F2_1_3</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>59091.25916721939</v>
+      </c>
+      <c r="F43" t="n">
+        <v>44318.44437541453</v>
+      </c>
+      <c r="G43" t="n">
+        <v>73864.07395902422</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>F1_1_1</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>1039028.169280454</v>
+      </c>
+      <c r="F44" t="n">
+        <v>779271.1269603405</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1298785.211600568</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>F1_1_2</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>5224997.977703433</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3918748.483277576</v>
+      </c>
+      <c r="G45" t="n">
+        <v>6531247.472129293</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>F1_1_3</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>5224997.977703433</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3918748.483277576</v>
+      </c>
+      <c r="G46" t="n">
+        <v>6531247.472129293</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>F2_1_1</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>47925.07986039567</v>
+      </c>
+      <c r="F47" t="n">
+        <v>35943.80989529676</v>
+      </c>
+      <c r="G47" t="n">
+        <v>59906.34982549458</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>F2_1_2</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>95850.15972079134</v>
+      </c>
+      <c r="F48" t="n">
+        <v>71887.61979059351</v>
+      </c>
+      <c r="G48" t="n">
+        <v>119812.6996509892</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>rp0250</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>F2_1_3</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>239625.3993019783</v>
+      </c>
+      <c r="F49" t="n">
+        <v>179719.0494764837</v>
+      </c>
+      <c r="G49" t="n">
+        <v>299531.7491274729</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>F1_1_1</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1292918.507796088</v>
+      </c>
+      <c r="F50" t="n">
+        <v>969688.8808470656</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1616148.13474511</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>F1_1_2</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>6501745.369664233</v>
+      </c>
+      <c r="F51" t="n">
+        <v>4876309.027248176</v>
+      </c>
+      <c r="G51" t="n">
+        <v>8127181.712080293</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>F1_1_3</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>6501745.369664233</v>
+      </c>
+      <c r="F52" t="n">
+        <v>4876309.027248176</v>
+      </c>
+      <c r="G52" t="n">
+        <v>8127181.712080293</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>F2_1_1</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>78854.55036974174</v>
+      </c>
+      <c r="F53" t="n">
+        <v>59140.91277730631</v>
+      </c>
+      <c r="G53" t="n">
+        <v>98568.1879621772</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>F2_1_2</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>157709.1007394835</v>
+      </c>
+      <c r="F54" t="n">
+        <v>118281.8255546126</v>
+      </c>
+      <c r="G54" t="n">
+        <v>197136.3759243544</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>rp0500</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>F2_1_3</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>394272.7518487088</v>
+      </c>
+      <c r="F55" t="n">
+        <v>295704.5638865315</v>
+      </c>
+      <c r="G55" t="n">
+        <v>492840.9398108859</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>rp1000</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>substation</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>substation</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>5564925.756320233</v>
-      </c>
-      <c r="F21" t="n">
-        <v>4173694.317240175</v>
-      </c>
-      <c r="G21" t="n">
-        <v>6956157.195400292</v>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>F1_1_1</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>1643862.4105116</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1232896.8078837</v>
+      </c>
+      <c r="G56" t="n">
+        <v>2054828.013139501</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>rp1000</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>F1_1_2</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>8266549.478147414</v>
+      </c>
+      <c r="F57" t="n">
+        <v>6199912.108610562</v>
+      </c>
+      <c r="G57" t="n">
+        <v>10333186.84768427</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>rp1000</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>F1_1_3</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>plant</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>8266549.478147414</v>
+      </c>
+      <c r="F58" t="n">
+        <v>6199912.108610562</v>
+      </c>
+      <c r="G58" t="n">
+        <v>10333186.84768427</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>rp1000</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>F2_1_1</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>105127.3619160917</v>
+      </c>
+      <c r="F59" t="n">
+        <v>78845.52143706879</v>
+      </c>
+      <c r="G59" t="n">
+        <v>131409.2023951146</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>rp1000</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>F2_1_2</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>210254.7238321834</v>
+      </c>
+      <c r="F60" t="n">
+        <v>157691.0428741376</v>
+      </c>
+      <c r="G60" t="n">
+        <v>262818.4047902293</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>rp1000</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>F2_1_3</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>substation</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>525636.8095804586</v>
+      </c>
+      <c r="F61" t="n">
+        <v>394227.6071853439</v>
+      </c>
+      <c r="G61" t="n">
+        <v>657046.011975573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>